<commit_message>
first and myexcel lines added
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -16,9 +16,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>mahima</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
+  <si>
+    <t>changes</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">excel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">as </t>
+  </si>
+  <si>
+    <t>well</t>
+  </si>
+  <si>
+    <t>more</t>
   </si>
 </sst>
 </file>
@@ -34,12 +58,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -54,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,15 +381,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="O8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="S10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="L13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="16:16">
+      <c r="P19" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
direct commit without staging area
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -49,10 +49,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,9 +91,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,7 +392,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -413,7 +421,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -423,7 +431,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -439,6 +447,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>